<commit_message>
- Font Size Correction - Resrouce file color changed from blue to appThemeColor - Next button from the Quiz page removed - Category display according their length of the string
</commit_message>
<xml_diff>
--- a/Java8_Questions.xlsx
+++ b/Java8_Questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
   <si>
     <t>Questions</t>
   </si>
@@ -517,6 +517,36 @@
  }
 }
 What is the output?</t>
+  </si>
+  <si>
+    <t>How would you write the following code using "Method References" in Java8?
+obj-&gt; obj.toString();</t>
+  </si>
+  <si>
+    <t>Object::toString</t>
+  </si>
+  <si>
+    <t>obj::toString</t>
+  </si>
+  <si>
+    <t>(Object)-&gt;toString()</t>
+  </si>
+  <si>
+    <t>How would you write the following code using "Method References" in Java8?
+()-&gt; obj.toString();</t>
+  </si>
+  <si>
+    <t>Object::new()
+What would be Lambda equivalent code to the above statement?</t>
+  </si>
+  <si>
+    <t>()-&gt;new Object()</t>
+  </si>
+  <si>
+    <t>(Object obj)-&gt;new Object()</t>
+  </si>
+  <si>
+    <t>(obj)-&gt; new Object()</t>
   </si>
 </sst>
 </file>
@@ -890,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1436,6 +1466,57 @@
       </c>
       <c r="E32" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Questions for Java8
</commit_message>
<xml_diff>
--- a/Java8_Questions.xlsx
+++ b/Java8_Questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="122">
   <si>
     <t>Questions</t>
   </si>
@@ -398,9 +398,6 @@
     <t>Default methods introduced in Java8 are also known as ____________ methods.</t>
   </si>
   <si>
-    <t>Extension</t>
-  </si>
-  <si>
     <t>Implicit</t>
   </si>
   <si>
@@ -547,6 +544,110 @@
   </si>
   <si>
     <t>(obj)-&gt; new Object()</t>
+  </si>
+  <si>
+    <t>What is the output of the following program?
+public static void testSyntax(String... args) {
+     Object o = () -&gt; System.out.println("Howdy, world!");
+     System.out.println(o.getClass());
+   }</t>
+  </si>
+  <si>
+    <t>java.lang.Object</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>public class TestLambda {
+ Runnable  testRunnable = ()-&gt;System.out.println(this.toString());;
+ public String toString() {
+  return "Test.toString()";
+ }
+ public static void main(String[] args) {
+  TestLambda l = new TestLambda();
+  l.testRunnable.run();
+ }
+}
+What is the output of the program?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test.toString()
+</t>
+  </si>
+  <si>
+    <t>TestLambda$Runnable…</t>
+  </si>
+  <si>
+    <t>public class TestLambda {
+ Runnable testInnerClassRunnable = new Runnable() {
+  public void run() {
+   System.out.println(this.toString());
+  }
+  public String toString() {
+   return "Test.Runnable.toString()";
+  };
+ };
+ Runnable  testLambdaRunnable = ()-&gt;System.out.println(this.toString());;
+ public String toString() {
+  return "Test.toString()";
+ }
+ public static void main(String[] args) {
+  TestLambda l = new TestLambda();
+  l.testInnerClassRunnable.run();
+  l.testLambdaRunnable.run();
+ }
+}
+What is the output of the program?</t>
+  </si>
+  <si>
+    <t>Test.Runnable.toString()
+Test.toString()</t>
+  </si>
+  <si>
+    <t>Test.Runnable.toString()</t>
+  </si>
+  <si>
+    <t>Extension/Virtual Extension</t>
+  </si>
+  <si>
+    <t>Stream&lt;String&gt; stringStream = Stream.of("Hello","World!");
+  System.out.println(stringStream.reduce("", String::concat));
+What is the output of the above program?</t>
+  </si>
+  <si>
+    <t>HelloWorld!</t>
+  </si>
+  <si>
+    <t>Hello World!</t>
+  </si>
+  <si>
+    <t>Stream&lt;String&gt; stringStream = Stream.of("Hello","World!");
+  BinaryOperator&lt;String&gt; strCustomConcat = (a,b) -&gt; {return a + " " + b;};
+  System.out.println(stringStream.reduce("", strCustomConcat));
+What is the output of the above program?</t>
+  </si>
+  <si>
+    <t>" Hello World!"</t>
+  </si>
+  <si>
+    <t>"Hello World!"</t>
+  </si>
+  <si>
+    <t>" Hello World! "</t>
+  </si>
+  <si>
+    <t>BinaryOperator&lt;String&gt; strCustomConcat = (a,b) -&gt; {return a + " " + b;};
+What would equivalent to the above code?</t>
+  </si>
+  <si>
+    <t>BinaryOperator&lt;String&gt; strCustomConcat = (String a,String b) -&gt; {return a + " " + b;};</t>
+  </si>
+  <si>
+    <t>BinaryOperator&lt;String&gt; strCustomConcat = (String a, b) -&gt; {return a + " " + b;};</t>
+  </si>
+  <si>
+    <t>BinaryOperator&lt;String&gt; strCustomConcat = (a, String b) -&gt; {return a + " " + b;};</t>
   </si>
 </sst>
 </file>
@@ -920,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1354,13 +1455,13 @@
         <v>72</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>50</v>
@@ -1368,33 +1469,33 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>21</v>
@@ -1402,16 +1503,16 @@
     </row>
     <row r="29" spans="1:5" ht="132" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>21</v>
@@ -1419,30 +1520,30 @@
     </row>
     <row r="30" spans="1:5" ht="132" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="180" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>21</v>
@@ -1453,13 +1554,13 @@
     </row>
     <row r="32" spans="1:5" ht="228" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="3">
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>21</v>
@@ -1470,16 +1571,16 @@
     </row>
     <row r="33" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>50</v>
@@ -1487,16 +1588,16 @@
     </row>
     <row r="34" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>50</v>
@@ -1504,18 +1605,120 @@
     </row>
     <row r="35" spans="1:5" ht="36" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="72" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="B36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="132" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="240" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="72" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="36" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>